<commit_message>
Fixed flags typo of 'NC----' instead of 'NZC---" (8 instances).
</commit_message>
<xml_diff>
--- a/6502_OpcodeMatrix.xlsx
+++ b/6502_OpcodeMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Sultan\Abacus\dev\scripts\k6502\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B7859-594E-4F4B-A924-F7AA7CFC403C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF4D832-6B90-40F7-95D0-89CACD87F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{A5E2A2B9-77CB-469B-8A6A-2146D12C11D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{A5E2A2B9-77CB-469B-8A6A-2146D12C11D1}"/>
   </bookViews>
   <sheets>
     <sheet name="6502_OpcodeMatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="323">
   <si>
     <t>6502 OPCODE MATRIX</t>
   </si>
@@ -713,9 +713,6 @@
   </si>
   <si>
     <t>NZC--V</t>
-  </si>
-  <si>
-    <t>NC----</t>
   </si>
   <si>
     <t>NZC---</t>
@@ -1541,9 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C88A6A-9F9D-46EF-8A5C-27EE186E6906}">
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1567,7 +1562,7 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I2" s="16"/>
     </row>
@@ -1579,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>3</v>
@@ -1588,16 +1583,16 @@
         <v>6</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1619,10 +1614,10 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -1644,10 +1639,10 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1669,10 +1664,10 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1694,10 +1689,10 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1719,10 +1714,10 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1744,10 +1739,10 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -1769,10 +1764,10 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -1794,10 +1789,10 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -1819,10 +1814,10 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -1848,10 +1843,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -1875,10 +1870,10 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -1900,10 +1895,10 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1925,10 +1920,10 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
@@ -1950,10 +1945,10 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -1977,10 +1972,10 @@
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -2004,10 +1999,10 @@
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -2029,10 +2024,10 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -2054,10 +2049,10 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -2079,10 +2074,10 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
@@ -2104,10 +2099,10 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -2129,10 +2124,10 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -2154,10 +2149,10 @@
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
@@ -2179,10 +2174,10 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -2204,10 +2199,10 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
       <c r="H28" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -2229,10 +2224,10 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -2254,10 +2249,10 @@
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
@@ -2279,10 +2274,10 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
@@ -2304,10 +2299,10 @@
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I32" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -2333,10 +2328,10 @@
         <v>1</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
@@ -2360,10 +2355,10 @@
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
@@ -2385,10 +2380,10 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
@@ -2410,10 +2405,10 @@
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
@@ -2435,10 +2430,10 @@
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
@@ -2462,10 +2457,10 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
@@ -2489,10 +2484,10 @@
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="12" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -2514,10 +2509,10 @@
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I40" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2539,10 +2534,10 @@
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="I41" s="18" t="s">
         <v>276</v>
-      </c>
-      <c r="I41" s="18" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2564,10 +2559,10 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I42" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2589,10 +2584,10 @@
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I43" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2614,10 +2609,10 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2639,10 +2634,10 @@
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I45" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2664,10 +2659,10 @@
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I46" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2689,10 +2684,10 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2714,10 +2709,10 @@
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I48" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -2739,10 +2734,10 @@
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I49" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -2764,10 +2759,10 @@
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -2793,10 +2788,10 @@
         <v>1</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I51" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
@@ -2820,10 +2815,10 @@
       </c>
       <c r="G52" s="13"/>
       <c r="H52" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I52" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -2845,10 +2840,10 @@
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
       <c r="H53" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
@@ -2870,10 +2865,10 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
@@ -2895,10 +2890,10 @@
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I55" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -2922,10 +2917,10 @@
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I56" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -2949,10 +2944,10 @@
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I57" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
@@ -2974,10 +2969,10 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
@@ -2999,10 +2994,10 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -3027,7 +3022,7 @@
         <v>225</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -3052,7 +3047,7 @@
         <v>225</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
@@ -3074,10 +3069,10 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
@@ -3099,10 +3094,10 @@
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
@@ -3127,7 +3122,7 @@
         <v>225</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
@@ -3149,10 +3144,10 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
@@ -3174,10 +3169,10 @@
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="H66" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
@@ -3202,7 +3197,7 @@
         <v>225</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
@@ -3224,10 +3219,10 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I68" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
@@ -3253,10 +3248,10 @@
         <v>1</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
@@ -3281,7 +3276,7 @@
         <v>225</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
@@ -3306,7 +3301,7 @@
         <v>225</v>
       </c>
       <c r="I71" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
@@ -3328,10 +3323,10 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I72" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
@@ -3353,10 +3348,10 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I73" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
@@ -3381,7 +3376,7 @@
         <v>225</v>
       </c>
       <c r="I74" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
@@ -3406,7 +3401,7 @@
         <v>225</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
@@ -3428,10 +3423,10 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I76" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
@@ -3453,10 +3448,10 @@
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
       <c r="H77" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
@@ -3478,10 +3473,10 @@
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
       <c r="H78" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
@@ -3503,10 +3498,10 @@
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
       <c r="H79" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
@@ -3528,10 +3523,10 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I80" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
@@ -3553,10 +3548,10 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I81" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
@@ -3578,10 +3573,10 @@
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
       <c r="H82" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
@@ -3603,10 +3598,10 @@
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
       <c r="H83" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
@@ -3628,10 +3623,10 @@
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
       <c r="H84" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I84" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
@@ -3653,10 +3648,10 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I85" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
@@ -3678,10 +3673,10 @@
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
       <c r="H86" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I86" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
@@ -3703,10 +3698,10 @@
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
       <c r="H87" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I87" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
@@ -3728,10 +3723,10 @@
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
       <c r="H88" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I88" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
@@ -3753,10 +3748,10 @@
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
       <c r="H89" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I89" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
@@ -3778,10 +3773,10 @@
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
       <c r="H90" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I90" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
@@ -3803,10 +3798,10 @@
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I91" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
@@ -3828,10 +3823,10 @@
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
       <c r="H92" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I92" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
@@ -3853,10 +3848,10 @@
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
       <c r="H93" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I93" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
@@ -3878,10 +3873,10 @@
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
       <c r="H94" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I94" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
@@ -3903,10 +3898,10 @@
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
       <c r="H95" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I95" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
@@ -3928,10 +3923,10 @@
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
       <c r="H96" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I96" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
@@ -3953,10 +3948,10 @@
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I97" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
@@ -3978,10 +3973,10 @@
       <c r="F98" s="15"/>
       <c r="G98" s="15"/>
       <c r="H98" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I98" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
@@ -4003,10 +3998,10 @@
       <c r="F99" s="15"/>
       <c r="G99" s="15"/>
       <c r="H99" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I99" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
@@ -4028,10 +4023,10 @@
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
       <c r="H100" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I100" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
@@ -4053,10 +4048,10 @@
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
       <c r="H101" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I101" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
@@ -4078,10 +4073,10 @@
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
       <c r="H102" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I102" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
@@ -4103,10 +4098,10 @@
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="H103" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I103" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
@@ -4128,10 +4123,10 @@
       <c r="F104" s="15"/>
       <c r="G104" s="15"/>
       <c r="H104" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I104" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
@@ -4153,10 +4148,10 @@
       <c r="F105" s="15"/>
       <c r="G105" s="15"/>
       <c r="H105" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I105" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
@@ -4178,10 +4173,10 @@
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="H106" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I106" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.45">
@@ -4207,10 +4202,10 @@
         <v>1</v>
       </c>
       <c r="H107" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I107" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.45">
@@ -4234,10 +4229,10 @@
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I108" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.45">
@@ -4259,10 +4254,10 @@
       <c r="F109" s="15"/>
       <c r="G109" s="15"/>
       <c r="H109" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I109" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.45">
@@ -4284,10 +4279,10 @@
       <c r="F110" s="15"/>
       <c r="G110" s="15"/>
       <c r="H110" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I110" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.45">
@@ -4309,10 +4304,10 @@
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
       <c r="H111" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I111" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.45">
@@ -4334,10 +4329,10 @@
       <c r="F112" s="10"/>
       <c r="G112" s="10"/>
       <c r="H112" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="I112" s="17" t="s">
         <v>249</v>
-      </c>
-      <c r="I112" s="17" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.45">
@@ -4361,10 +4356,10 @@
       </c>
       <c r="G113" s="15"/>
       <c r="H113" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I113" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.45">
@@ -4386,10 +4381,10 @@
       <c r="F114" s="9"/>
       <c r="G114" s="9"/>
       <c r="H114" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I114" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.45">
@@ -4413,10 +4408,10 @@
       </c>
       <c r="G115" s="15"/>
       <c r="H115" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I115" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.45">
@@ -4440,10 +4435,10 @@
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I116" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.45">
@@ -4467,10 +4462,10 @@
       </c>
       <c r="G117" s="9"/>
       <c r="H117" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I117" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.45">
@@ -4492,10 +4487,10 @@
       <c r="F118" s="15"/>
       <c r="G118" s="15"/>
       <c r="H118" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I118" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.45">
@@ -4517,10 +4512,10 @@
       <c r="F119" s="13"/>
       <c r="G119" s="13"/>
       <c r="H119" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I119" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.45">
@@ -4542,10 +4537,10 @@
       <c r="F120" s="15"/>
       <c r="G120" s="15"/>
       <c r="H120" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I120" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.45">
@@ -4567,10 +4562,10 @@
       <c r="F121" s="13"/>
       <c r="G121" s="13"/>
       <c r="H121" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I121" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.45">
@@ -4592,10 +4587,10 @@
       <c r="F122" s="9"/>
       <c r="G122" s="9"/>
       <c r="H122" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I122" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.45">
@@ -4617,10 +4612,10 @@
       <c r="F123" s="9"/>
       <c r="G123" s="9"/>
       <c r="H123" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I123" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.45">
@@ -4642,10 +4637,10 @@
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
       <c r="H124" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I124" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.45">
@@ -4667,10 +4662,10 @@
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
       <c r="H125" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="I125" s="18" t="s">
         <v>254</v>
-      </c>
-      <c r="I125" s="18" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.45">
@@ -4692,10 +4687,10 @@
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
       <c r="H126" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I126" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.45">
@@ -4717,10 +4712,10 @@
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
       <c r="H127" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I127" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.45">
@@ -4742,10 +4737,10 @@
       <c r="F128" s="9"/>
       <c r="G128" s="9"/>
       <c r="H128" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I128" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.45">
@@ -4771,10 +4766,10 @@
         <v>1</v>
       </c>
       <c r="H129" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I129" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.45">
@@ -4798,10 +4793,10 @@
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I130" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.45">
@@ -4823,10 +4818,10 @@
       <c r="F131" s="15"/>
       <c r="G131" s="15"/>
       <c r="H131" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I131" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.45">
@@ -4848,10 +4843,10 @@
       <c r="F132" s="9"/>
       <c r="G132" s="9"/>
       <c r="H132" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I132" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.45">
@@ -4873,10 +4868,10 @@
       <c r="F133" s="10"/>
       <c r="G133" s="10"/>
       <c r="H133" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="I133" s="17" t="s">
         <v>247</v>
-      </c>
-      <c r="I133" s="17" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.45">
@@ -4900,10 +4895,10 @@
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I134" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.45">
@@ -4927,10 +4922,10 @@
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I135" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.45">
@@ -4952,10 +4947,10 @@
       <c r="F136" s="9"/>
       <c r="G136" s="9"/>
       <c r="H136" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I136" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.45">
@@ -4973,10 +4968,10 @@
       <c r="F137" s="9"/>
       <c r="G137" s="9"/>
       <c r="H137" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I137" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.45">
@@ -5001,7 +4996,7 @@
         <v>225</v>
       </c>
       <c r="I138" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5026,7 +5021,7 @@
         <v>225</v>
       </c>
       <c r="I139" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5048,10 +5043,10 @@
       <c r="F140" s="9"/>
       <c r="G140" s="9"/>
       <c r="H140" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I140" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5073,10 +5068,10 @@
       <c r="F141" s="15"/>
       <c r="G141" s="15"/>
       <c r="H141" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I141" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5101,7 +5096,7 @@
         <v>225</v>
       </c>
       <c r="I142" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="143" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5123,10 +5118,10 @@
       <c r="F143" s="15"/>
       <c r="G143" s="15"/>
       <c r="H143" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I143" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5144,10 +5139,10 @@
       <c r="F144" s="9"/>
       <c r="G144" s="9"/>
       <c r="H144" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I144" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="145" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5172,7 +5167,7 @@
         <v>225</v>
       </c>
       <c r="I145" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="146" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5194,10 +5189,10 @@
       <c r="F146" s="9"/>
       <c r="G146" s="9"/>
       <c r="H146" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I146" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="147" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5223,10 +5218,10 @@
         <v>1</v>
       </c>
       <c r="H147" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I147" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="148" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5253,7 +5248,7 @@
         <v>225</v>
       </c>
       <c r="I148" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5278,7 +5273,7 @@
         <v>225</v>
       </c>
       <c r="I149" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="150" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5300,10 +5295,10 @@
       <c r="F150" s="9"/>
       <c r="G150" s="9"/>
       <c r="H150" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I150" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="151" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5325,10 +5320,10 @@
       <c r="F151" s="15"/>
       <c r="G151" s="15"/>
       <c r="H151" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I151" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="152" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5355,7 +5350,7 @@
         <v>225</v>
       </c>
       <c r="I152" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5382,7 +5377,7 @@
         <v>225</v>
       </c>
       <c r="I153" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -5404,10 +5399,10 @@
       <c r="F154" s="9"/>
       <c r="G154" s="9"/>
       <c r="H154" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I154" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5424,7 +5419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E86595-4739-429A-8A61-241B869484CE}">
   <dimension ref="A2:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -5440,10 +5435,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>296</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -5451,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -5459,15 +5454,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -5475,7 +5470,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -5483,23 +5478,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -5507,23 +5502,23 @@
         <v>5</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>308</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -5531,7 +5526,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -5539,7 +5534,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -5547,7 +5542,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -5555,7 +5550,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -5563,7 +5558,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -5571,7 +5566,7 @@
         <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -5579,7 +5574,7 @@
         <v>174</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -5587,7 +5582,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -5595,7 +5590,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
@@ -5603,7 +5598,7 @@
         <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
@@ -5611,7 +5606,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
@@ -5619,7 +5614,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
@@ -5627,17 +5622,17 @@
         <v>219</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>